<commit_message>
wyniki 200 epok f10.
</commit_message>
<xml_diff>
--- a/distributions/distribution_f10_1p.xlsx
+++ b/distributions/distribution_f10_1p.xlsx
@@ -442,42 +442,42 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.09866071428571428</v>
+        <v>0.1633928571428571</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3794642857142857</v>
+        <v>0.5102678571428572</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.621875</v>
+        <v>0.7857142857142858</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.8026785714285714</v>
+        <v>0.9178571428571429</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.9191964285714285</v>
+        <v>0.9651785714285714</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.9732142857142856</v>
+        <v>0.9897321428571428</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9937499999999999</v>
+        <v>0.9977678571428571</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.9982142857142856</v>
+        <v>0.9986607142857142</v>
       </c>
     </row>
     <row r="10">
@@ -557,17 +557,17 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.9995535714285715</v>
+        <v>0.9991071428571429</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.9995535714285715</v>
+        <v>0.9991071428571429</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.9995535714285715</v>
+        <v>0.9991071428571429</v>
       </c>
     </row>
     <row r="28">

</xml_diff>